<commit_message>
feature: add test amount
</commit_message>
<xml_diff>
--- a/testcase_result.xlsx
+++ b/testcase_result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,12 +536,32 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>GA Image</t>
+          <t>GA Image 1</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>ACO Image</t>
+          <t>ACO Image 1</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>GA Image 2</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>ACO Image 2</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>GA Image 3</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>ACO Image 3</t>
         </is>
       </c>
     </row>
@@ -575,31 +595,67 @@
       <c r="I2" t="n">
         <v>102.1070184418289</v>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="J2" t="n">
+        <v>102.1070184418289</v>
+      </c>
+      <c r="K2" t="n">
+        <v>104.0130965649983</v>
+      </c>
       <c r="L2" t="n">
         <v>104.0130965649983</v>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>104.0130965649983</v>
+      </c>
+      <c r="N2" t="n">
+        <v>104.0130965649983</v>
+      </c>
       <c r="O2" t="n">
-        <v>0.0012</v>
-      </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
+        <v>0.001</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.0008</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.0009</v>
+      </c>
       <c r="R2" t="n">
         <v>0.0008</v>
       </c>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
+      <c r="S2" t="n">
+        <v>0.0008</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.0008</v>
+      </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>./imageResult/t5_GA_10.png</t>
+          <t>./imageResult/t5_1_GA_10.png</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>./imageResult/t5_ACO_10.png</t>
+          <t>./imageResult/t5_1_ACO_10.png</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_GA_10.png</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_ACO_10.png</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_GA_10.png</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_ACO_10.png</t>
         </is>
       </c>
     </row>
@@ -633,31 +689,67 @@
       <c r="I3" t="n">
         <v>102.1070184418289</v>
       </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>102.1070184418289</v>
+      </c>
+      <c r="K3" t="n">
+        <v>102.1070184418289</v>
+      </c>
       <c r="L3" t="n">
         <v>104.0130965649983</v>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>104.0130965649983</v>
+      </c>
+      <c r="N3" t="n">
+        <v>104.0130965649983</v>
+      </c>
       <c r="O3" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
+        <v>0.0009</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.0009</v>
+      </c>
       <c r="R3" t="n">
         <v>0.0009</v>
       </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
+      <c r="S3" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.0009</v>
+      </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>./imageResult/t5_GA_50.png</t>
+          <t>./imageResult/t5_1_GA_50.png</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>./imageResult/t5_ACO_50.png</t>
+          <t>./imageResult/t5_1_ACO_50.png</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_GA_50.png</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_ACO_50.png</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_GA_50.png</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_ACO_50.png</t>
         </is>
       </c>
     </row>
@@ -691,31 +783,67 @@
       <c r="I4" t="n">
         <v>102.1070184418289</v>
       </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>102.1070184418289</v>
+      </c>
+      <c r="K4" t="n">
+        <v>102.1070184418289</v>
+      </c>
       <c r="L4" t="n">
         <v>104.0130965649983</v>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>104.0130965649983</v>
+      </c>
+      <c r="N4" t="n">
+        <v>104.0130965649983</v>
+      </c>
       <c r="O4" t="n">
-        <v>0.0012</v>
-      </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
+        <v>0.0011</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.0011</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.0011</v>
+      </c>
       <c r="R4" t="n">
         <v>0.001</v>
       </c>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
+      <c r="S4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.001</v>
+      </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>./imageResult/t5_GA_100.png</t>
+          <t>./imageResult/t5_1_GA_100.png</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>./imageResult/t5_ACO_100.png</t>
+          <t>./imageResult/t5_1_ACO_100.png</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_GA_100.png</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_ACO_100.png</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_GA_100.png</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>./imageResult/t5_2_ACO_100.png</t>
         </is>
       </c>
     </row>
@@ -747,33 +875,69 @@
         <v>10</v>
       </c>
       <c r="I5" t="n">
-        <v>43.64254224345727</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+        <v>49.42117558688741</v>
+      </c>
+      <c r="J5" t="n">
+        <v>46.26525516106483</v>
+      </c>
+      <c r="K5" t="n">
+        <v>46.81591122239789</v>
+      </c>
       <c r="L5" t="n">
         <v>31.88252949105588</v>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>31.22691510942754</v>
+      </c>
+      <c r="N5" t="n">
+        <v>31.88252949105588</v>
+      </c>
       <c r="O5" t="n">
         <v>0.0011</v>
       </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0.0011</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.0011</v>
+      </c>
       <c r="R5" t="n">
         <v>0.0009</v>
       </c>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
+      <c r="S5" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.001</v>
+      </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>./imageResult/burma14_GA_10.png</t>
+          <t>./imageResult/burma14_1_GA_10.png</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>./imageResult/burma14_ACO_10.png</t>
+          <t>./imageResult/burma14_1_ACO_10.png</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_GA_10.png</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_ACO_10.png</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_GA_10.png</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_ACO_10.png</t>
         </is>
       </c>
     </row>
@@ -805,33 +969,69 @@
         <v>10</v>
       </c>
       <c r="I6" t="n">
-        <v>42.72460933397221</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+        <v>37.67518177401836</v>
+      </c>
+      <c r="J6" t="n">
+        <v>37.07000077260059</v>
+      </c>
+      <c r="K6" t="n">
+        <v>37.08847053051498</v>
+      </c>
       <c r="L6" t="n">
+        <v>31.22691510942754</v>
+      </c>
+      <c r="M6" t="n">
+        <v>31.22691510942754</v>
+      </c>
+      <c r="N6" t="n">
         <v>31.88252949105588</v>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
       <c r="O6" t="n">
         <v>0.0022</v>
       </c>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>0.0023</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.0022</v>
+      </c>
       <c r="R6" t="n">
         <v>0.0016</v>
       </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
+      <c r="S6" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.0018</v>
+      </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>./imageResult/burma14_GA_50.png</t>
+          <t>./imageResult/burma14_1_GA_50.png</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>./imageResult/burma14_ACO_50.png</t>
+          <t>./imageResult/burma14_1_ACO_50.png</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_GA_50.png</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_ACO_50.png</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_GA_50.png</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_ACO_50.png</t>
         </is>
       </c>
     </row>
@@ -863,33 +1063,69 @@
         <v>10</v>
       </c>
       <c r="I7" t="n">
-        <v>42.27229592389322</v>
-      </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+        <v>36.0214184683452</v>
+      </c>
+      <c r="J7" t="n">
+        <v>34.86174060408727</v>
+      </c>
+      <c r="K7" t="n">
+        <v>33.46723944553786</v>
+      </c>
       <c r="L7" t="n">
         <v>31.22691510942754</v>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>31.45623383762054</v>
+      </c>
+      <c r="N7" t="n">
+        <v>31.88252949105588</v>
+      </c>
       <c r="O7" t="n">
         <v>0.0035</v>
       </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0.0038</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.0034</v>
+      </c>
       <c r="R7" t="n">
+        <v>0.0024</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.0028</v>
+      </c>
+      <c r="T7" t="n">
         <v>0.0025</v>
       </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr">
         <is>
-          <t>./imageResult/burma14_GA_100.png</t>
+          <t>./imageResult/burma14_1_GA_100.png</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>./imageResult/burma14_ACO_100.png</t>
+          <t>./imageResult/burma14_1_ACO_100.png</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_GA_100.png</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_ACO_100.png</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_GA_100.png</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>./imageResult/burma14_2_ACO_100.png</t>
         </is>
       </c>
     </row>
@@ -921,33 +1157,69 @@
         <v>10</v>
       </c>
       <c r="I8" t="n">
-        <v>562285.6447819617</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+        <v>554427.2997867422</v>
+      </c>
+      <c r="J8" t="n">
+        <v>568444.5940621259</v>
+      </c>
+      <c r="K8" t="n">
+        <v>583017.4756071992</v>
+      </c>
       <c r="L8" t="n">
-        <v>48527.92247208483</v>
-      </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+        <v>49294.74163904427</v>
+      </c>
+      <c r="M8" t="n">
+        <v>49215.61251916289</v>
+      </c>
+      <c r="N8" t="n">
+        <v>49143.7729793856</v>
+      </c>
       <c r="O8" t="n">
+        <v>0.008699999999999999</v>
+      </c>
+      <c r="P8" t="n">
         <v>0.008500000000000001</v>
       </c>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
+      <c r="Q8" t="n">
+        <v>0.008500000000000001</v>
+      </c>
       <c r="R8" t="n">
+        <v>0.0674</v>
+      </c>
+      <c r="S8" t="n">
         <v>0.0665</v>
       </c>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
+      <c r="T8" t="n">
+        <v>0.0679</v>
+      </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>./imageResult/lin318_GA_10.png</t>
+          <t>./imageResult/lin318_1_GA_10.png</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>./imageResult/lin318_ACO_10.png</t>
+          <t>./imageResult/lin318_1_ACO_10.png</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_GA_10.png</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_ACO_10.png</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_GA_10.png</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_ACO_10.png</t>
         </is>
       </c>
     </row>
@@ -979,33 +1251,69 @@
         <v>10</v>
       </c>
       <c r="I9" t="n">
-        <v>534787.8149600039</v>
-      </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+        <v>511714.6596703269</v>
+      </c>
+      <c r="J9" t="n">
+        <v>540311.5082501203</v>
+      </c>
+      <c r="K9" t="n">
+        <v>533365.6925958826</v>
+      </c>
       <c r="L9" t="n">
-        <v>49143.7729793856</v>
-      </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
+        <v>48563.49026440229</v>
+      </c>
+      <c r="M9" t="n">
+        <v>48572.80330933771</v>
+      </c>
+      <c r="N9" t="n">
+        <v>49215.61251916289</v>
+      </c>
       <c r="O9" t="n">
-        <v>0.035</v>
-      </c>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
+        <v>0.0351</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.0351</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.0351</v>
+      </c>
       <c r="R9" t="n">
-        <v>0.3178</v>
-      </c>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
+        <v>0.3182</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.3186</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.3203</v>
+      </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>./imageResult/lin318_GA_50.png</t>
+          <t>./imageResult/lin318_1_GA_50.png</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>./imageResult/lin318_ACO_50.png</t>
+          <t>./imageResult/lin318_1_ACO_50.png</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_GA_50.png</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_ACO_50.png</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_GA_50.png</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_ACO_50.png</t>
         </is>
       </c>
     </row>
@@ -1037,33 +1345,69 @@
         <v>10</v>
       </c>
       <c r="I10" t="n">
-        <v>518955.5023980857</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+        <v>525354.1034295225</v>
+      </c>
+      <c r="J10" t="n">
+        <v>503198.0617196271</v>
+      </c>
+      <c r="K10" t="n">
+        <v>521017.7767133673</v>
+      </c>
       <c r="L10" t="n">
-        <v>48554.11488899639</v>
-      </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+        <v>48320.84193889733</v>
+      </c>
+      <c r="M10" t="n">
+        <v>48835.97530486222</v>
+      </c>
+      <c r="N10" t="n">
+        <v>48585.25741399533</v>
+      </c>
       <c r="O10" t="n">
-        <v>0.06900000000000001</v>
-      </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
+        <v>0.0701</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.0687</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.0697</v>
+      </c>
       <c r="R10" t="n">
-        <v>0.6301</v>
-      </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
+        <v>0.6375999999999999</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.6425</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.6393</v>
+      </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>./imageResult/lin318_GA_100.png</t>
+          <t>./imageResult/lin318_1_GA_100.png</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>./imageResult/lin318_ACO_100.png</t>
+          <t>./imageResult/lin318_1_ACO_100.png</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_GA_100.png</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_ACO_100.png</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_GA_100.png</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>./imageResult/lin318_2_ACO_100.png</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: add file dedicated to testcase
</commit_message>
<xml_diff>
--- a/testcase_result.xlsx
+++ b/testcase_result.xlsx
@@ -599,7 +599,7 @@
         <v>102.1070184418289</v>
       </c>
       <c r="K2" t="n">
-        <v>104.0130965649983</v>
+        <v>102.1070184418289</v>
       </c>
       <c r="L2" t="n">
         <v>104.0130965649983</v>
@@ -611,22 +611,22 @@
         <v>104.0130965649983</v>
       </c>
       <c r="O2" t="n">
-        <v>0.001</v>
+        <v>0.0011</v>
       </c>
       <c r="P2" t="n">
         <v>0.0008</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0009</v>
+        <v>0.0008</v>
       </c>
       <c r="R2" t="n">
         <v>0.0008</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0026</v>
+        <v>0.0008</v>
       </c>
       <c r="T2" t="n">
-        <v>0.0007</v>
+        <v>0.0016</v>
       </c>
       <c r="U2" t="inlineStr">
         <is>
@@ -705,16 +705,16 @@
         <v>104.0130965649983</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0009</v>
+        <v>0.001</v>
       </c>
       <c r="P3" t="n">
+        <v>0.0011</v>
+      </c>
+      <c r="Q3" t="n">
         <v>0.001</v>
       </c>
-      <c r="Q3" t="n">
-        <v>0.0009</v>
-      </c>
       <c r="R3" t="n">
-        <v>0.0009</v>
+        <v>0.001</v>
       </c>
       <c r="S3" t="n">
         <v>0.0009</v>
@@ -799,19 +799,19 @@
         <v>104.0130965649983</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0011</v>
+        <v>0.0013</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0011</v>
+        <v>0.0012</v>
       </c>
       <c r="Q4" t="n">
         <v>0.0011</v>
       </c>
       <c r="R4" t="n">
+        <v>0.0011</v>
+      </c>
+      <c r="S4" t="n">
         <v>0.001</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.0011</v>
       </c>
       <c r="T4" t="n">
         <v>0.001</v>
@@ -875,19 +875,19 @@
         <v>10</v>
       </c>
       <c r="I5" t="n">
-        <v>50.76352496678864</v>
+        <v>39.37213886457447</v>
       </c>
       <c r="J5" t="n">
-        <v>45.4099348702336</v>
+        <v>45.69297498377761</v>
       </c>
       <c r="K5" t="n">
-        <v>51.55699566478027</v>
+        <v>49.70847756767837</v>
       </c>
       <c r="L5" t="n">
         <v>31.22691510942754</v>
       </c>
       <c r="M5" t="n">
-        <v>31.88252949105588</v>
+        <v>31.22691510942754</v>
       </c>
       <c r="N5" t="n">
         <v>31.88252949105588</v>
@@ -899,13 +899,13 @@
         <v>0.0011</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0011</v>
+        <v>0.0012</v>
       </c>
       <c r="R5" t="n">
         <v>0.0009</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0009</v>
+        <v>0.001</v>
       </c>
       <c r="T5" t="n">
         <v>0.001</v>
@@ -969,40 +969,40 @@
         <v>10</v>
       </c>
       <c r="I6" t="n">
-        <v>37.15106686359928</v>
+        <v>37.00463120931033</v>
       </c>
       <c r="J6" t="n">
-        <v>44.8937944990004</v>
+        <v>44.27627586887465</v>
       </c>
       <c r="K6" t="n">
-        <v>39.6899265990123</v>
+        <v>41.01081695451413</v>
       </c>
       <c r="L6" t="n">
-        <v>31.22691510942754</v>
+        <v>31.88252949105588</v>
       </c>
       <c r="M6" t="n">
-        <v>31.88252949105588</v>
+        <v>32.11184821924887</v>
       </c>
       <c r="N6" t="n">
-        <v>31.88252949105588</v>
+        <v>31.45623383762054</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0022</v>
+        <v>0.0021</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0022</v>
+        <v>0.0023</v>
       </c>
       <c r="Q6" t="n">
         <v>0.0023</v>
       </c>
       <c r="R6" t="n">
+        <v>0.0018</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.0017</v>
+      </c>
+      <c r="T6" t="n">
         <v>0.0016</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.0018</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0.0017</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
@@ -1063,16 +1063,16 @@
         <v>10</v>
       </c>
       <c r="I7" t="n">
-        <v>34.83039736354373</v>
+        <v>42.19843329089865</v>
       </c>
       <c r="J7" t="n">
-        <v>43.35471087658466</v>
+        <v>40.31098556893893</v>
       </c>
       <c r="K7" t="n">
-        <v>36.56324197122565</v>
+        <v>42.57832116775565</v>
       </c>
       <c r="L7" t="n">
-        <v>32.11184821924887</v>
+        <v>31.88252949105588</v>
       </c>
       <c r="M7" t="n">
         <v>31.88252949105588</v>
@@ -1081,7 +1081,7 @@
         <v>31.22691510942754</v>
       </c>
       <c r="O7" t="n">
-        <v>0.0035</v>
+        <v>0.0041</v>
       </c>
       <c r="P7" t="n">
         <v>0.0035</v>
@@ -1157,40 +1157,40 @@
         <v>10</v>
       </c>
       <c r="I8" t="n">
-        <v>551695.2621313389</v>
+        <v>560654.4810176021</v>
       </c>
       <c r="J8" t="n">
-        <v>563773.6720051733</v>
+        <v>572266.7876941945</v>
       </c>
       <c r="K8" t="n">
-        <v>560316.2805824048</v>
+        <v>565783.7988525628</v>
       </c>
       <c r="L8" t="n">
         <v>49143.7729793856</v>
       </c>
       <c r="M8" t="n">
-        <v>49215.61251916289</v>
+        <v>49294.74163904427</v>
       </c>
       <c r="N8" t="n">
         <v>49215.61251916289</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0091</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="P8" t="n">
-        <v>0.0083</v>
+        <v>0.008399999999999999</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0086</v>
       </c>
       <c r="R8" t="n">
-        <v>0.068</v>
+        <v>0.0688</v>
       </c>
       <c r="S8" t="n">
-        <v>0.06569999999999999</v>
+        <v>0.06850000000000001</v>
       </c>
       <c r="T8" t="n">
-        <v>0.06610000000000001</v>
+        <v>0.0683</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
@@ -1251,40 +1251,40 @@
         <v>10</v>
       </c>
       <c r="I9" t="n">
-        <v>533921.932031111</v>
+        <v>535498.8765180835</v>
       </c>
       <c r="J9" t="n">
-        <v>541321.7020989901</v>
+        <v>535156.0096518323</v>
       </c>
       <c r="K9" t="n">
-        <v>533837.8675633604</v>
+        <v>530950.212590666</v>
       </c>
       <c r="L9" t="n">
-        <v>48382.86890044977</v>
+        <v>48359.58007325514</v>
       </c>
       <c r="M9" t="n">
-        <v>48382.86890044977</v>
+        <v>48350.55885416948</v>
       </c>
       <c r="N9" t="n">
-        <v>48382.86890044977</v>
+        <v>48554.11488899639</v>
       </c>
       <c r="O9" t="n">
-        <v>0.0335</v>
+        <v>0.0347</v>
       </c>
       <c r="P9" t="n">
-        <v>0.0337</v>
+        <v>0.0357</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.0342</v>
+        <v>0.0345</v>
       </c>
       <c r="R9" t="n">
-        <v>0.3146</v>
+        <v>0.331</v>
       </c>
       <c r="S9" t="n">
-        <v>0.316</v>
+        <v>0.3248</v>
       </c>
       <c r="T9" t="n">
-        <v>0.3163</v>
+        <v>0.3297</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
@@ -1345,40 +1345,40 @@
         <v>10</v>
       </c>
       <c r="I10" t="n">
-        <v>487818.0359691684</v>
+        <v>513333.8967455443</v>
       </c>
       <c r="J10" t="n">
-        <v>502701.7910008261</v>
+        <v>535586.108007305</v>
       </c>
       <c r="K10" t="n">
-        <v>523701.944058846</v>
+        <v>527628.7018299692</v>
       </c>
       <c r="L10" t="n">
-        <v>48108.8789343028</v>
+        <v>48928.00065664363</v>
       </c>
       <c r="M10" t="n">
         <v>48783.31682921913</v>
       </c>
       <c r="N10" t="n">
-        <v>49215.61251916289</v>
+        <v>49143.7729793856</v>
       </c>
       <c r="O10" t="n">
-        <v>0.0663</v>
+        <v>0.068</v>
       </c>
       <c r="P10" t="n">
-        <v>0.0663</v>
+        <v>0.0696</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.0675</v>
+        <v>0.0678</v>
       </c>
       <c r="R10" t="n">
-        <v>0.6301</v>
+        <v>0.6637999999999999</v>
       </c>
       <c r="S10" t="n">
-        <v>0.6429</v>
+        <v>0.6497000000000001</v>
       </c>
       <c r="T10" t="n">
-        <v>0.6337</v>
+        <v>0.6545</v>
       </c>
       <c r="U10" t="inlineStr">
         <is>

</xml_diff>